<commit_message>
Fix Submodules TableDescription and recreate SQL scripts
</commit_message>
<xml_diff>
--- a/R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx
+++ b/R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="frontend_table_description" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="table_description" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -511,8 +511,8 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fill retrol. MRP Evaluaton study_phase and ward_name by encounter
</commit_message>
<xml_diff>
--- a/R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx
+++ b/R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx
@@ -103,13 +103,13 @@
     <t xml:space="preserve">ward_name</t>
   </si>
   <si>
-    <t xml:space="preserve">optional – Name of the ward where the patient was during the medication analysis</t>
+    <t xml:space="preserve">Name of the ward where the patient was during the medication analysis or the very first relevant ward</t>
   </si>
   <si>
     <t xml:space="preserve">study_phase</t>
   </si>
   <si>
-    <t xml:space="preserve">optional – Study phase („PhaseA“, „PhaseBTest“ or „PhaseB“); must be filled if meda_id is not empty</t>
+    <t xml:space="preserve">Study phase („PhaseA“, „PhaseBTest“ or „PhaseB“); must be filled if there was any contact with a observed ward in his medical case</t>
   </si>
   <si>
     <t xml:space="preserve">ret_id</t>
@@ -523,15 +523,15 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="77.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="98.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="56.44"/>
   </cols>

</xml_diff>

<commit_message>
Add ret_redcap_repeat_instance in dp_mrp_calculation
</commit_message>
<xml_diff>
--- a/R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx
+++ b/R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t xml:space="preserve">optional – Redcap ID of the generated retrolective_mrpbewertung_fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ret_redcap_repeat_instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optional – Redcap repeat instance id</t>
   </si>
   <si>
     <t xml:space="preserve">mrp_proxy_type</t>
@@ -523,11 +529,11 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.63"/>
@@ -695,7 +701,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="1" t="s">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -720,19 +727,29 @@
       <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="1048327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
     <row r="1048328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>